<commit_message>
add resources tab to rubric
</commit_message>
<xml_diff>
--- a/Lab3/Lab3_Rubric.xlsx
+++ b/Lab3/Lab3_Rubric.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickfontenot/Dropbox/Mac/Documents/GitHub/airbnb/airbnb/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBA0F5BD-5A6A-7E4B-A247-6F917F8DE6B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{566E56EC-35AF-3C47-9B88-3C165D2D5F72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" xr2:uid="{8F3C83E5-0E95-DF4A-B795-46D227A43409}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16180" activeTab="1" xr2:uid="{8F3C83E5-0E95-DF4A-B795-46D227A43409}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Resorces" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Category </t>
   </si>
@@ -174,6 +175,60 @@
   </si>
   <si>
     <t>All</t>
+  </si>
+  <si>
+    <t>Here's another NYC Map I used for VIZ:</t>
+  </si>
+  <si>
+    <t>Joseph Lazarus to Everyone (9:19 AM)</t>
+  </si>
+  <si>
+    <t>import pandas as pd</t>
+  </si>
+  <si>
+    <t>import plotly.express as px</t>
+  </si>
+  <si>
+    <t>fig = px.scatter_mapbox(df, lat="latitude", lon="longitude", color='multi_listings',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        hover_data=["host_name", "host_listings_count","neighbourhood_group_cleansed"],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        opacity = .1,zoom=10, height=500)</t>
+  </si>
+  <si>
+    <t>fig.update_layout(mapbox_style="open-street-map")</t>
+  </si>
+  <si>
+    <t>fig.update_layout(margin={"r":5,"t":5,"l":5,"b":5})</t>
+  </si>
+  <si>
+    <t>fig.show()</t>
+  </si>
+  <si>
+    <t>Joseph Lazarus to Everyone (9:27 AM)</t>
+  </si>
+  <si>
+    <t>tuning spectral clustering</t>
+  </si>
+  <si>
+    <t>https://towardsdatascience.com/spectral-graph-clustering-and-optimal-number-of-clusters-estimation-32704189afbe</t>
+  </si>
+  <si>
+    <t>https://plotly.com/python/scattermapbox/</t>
+  </si>
+  <si>
+    <t>^map plotting</t>
+  </si>
+  <si>
+    <t>Puri Rudick to Everyone (9:42 AM)</t>
+  </si>
+  <si>
+    <t>https://scikit-learn.org/stable/auto_examples/cluster/plot_kmeans_silhouette_analysis.html</t>
+  </si>
+  <si>
+    <t>Cool plot for silhouette</t>
   </si>
 </sst>
 </file>
@@ -583,8 +638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90DAF0E-865A-904C-9F67-2284D017278C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="68.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -786,6 +841,111 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3788E36-C944-1344-9685-3F389492D739}">
+  <dimension ref="A1:A21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DE16E19-11C8-1544-A1FD-B1AF0034DC30}">
   <dimension ref="A1:C8"/>
   <sheetViews>

</xml_diff>

<commit_message>
load to data to repo
</commit_message>
<xml_diff>
--- a/Lab3/Lab3_Rubric.xlsx
+++ b/Lab3/Lab3_Rubric.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rickfontenot/Dropbox/Mac/Documents/GitHub/airbnb/airbnb/Lab3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56FB4B2-11B2-EB47-9443-306D55938FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF42ED4-FA9E-1344-8FE0-D4D7143859A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="20640" windowHeight="16120" xr2:uid="{8F3C83E5-0E95-DF4A-B795-46D227A43409}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="20640" windowHeight="16080" xr2:uid="{8F3C83E5-0E95-DF4A-B795-46D227A43409}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -332,6 +331,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,15 +649,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A90DAF0E-865A-904C-9F67-2284D017278C}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="68.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="109.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="109.33203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -668,7 +668,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -684,13 +684,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="12">
         <v>10</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
@@ -698,9 +698,9 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="6" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -711,7 +711,7 @@
       <c r="B5" s="2">
         <v>10</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -722,7 +722,7 @@
       <c r="B6" s="2">
         <v>10</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -733,7 +733,7 @@
       <c r="B7" s="2">
         <v>10</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -744,7 +744,7 @@
       <c r="B8" s="2">
         <v>10</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -755,7 +755,7 @@
       <c r="B9" s="2">
         <v>10</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -766,7 +766,7 @@
       <c r="B10" s="2">
         <v>20</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
     </row>
@@ -777,7 +777,7 @@
       <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -788,7 +788,7 @@
       <c r="B12" s="2">
         <v>10</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
     </row>
@@ -796,10 +796,10 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="7">
+      <c r="B16" s="6">
         <v>44511</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>24</v>
       </c>
       <c r="D16" t="s">
@@ -810,10 +810,10 @@
       <c r="A17" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="6">
         <v>44518</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="D17" t="s">
@@ -824,10 +824,10 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="6">
         <v>44525</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -835,7 +835,7 @@
       <c r="A19" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="6">
         <v>44528</v>
       </c>
       <c r="D19" t="s">
@@ -922,7 +922,7 @@
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -969,90 +969,90 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="69.33203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="6" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="69.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="22" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="10"/>
+      <c r="C1" s="9"/>
     </row>
     <row r="2" spans="1:3" ht="66" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="22" x14ac:dyDescent="0.25">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="22" x14ac:dyDescent="0.25">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="22" x14ac:dyDescent="0.25">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>4</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="44" x14ac:dyDescent="0.25">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>5</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="10"/>
+      <c r="C6" s="9"/>
     </row>
     <row r="7" spans="1:3" ht="22" x14ac:dyDescent="0.25">
-      <c r="A7" s="10">
+      <c r="A7" s="9">
         <v>6</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C7" s="10"/>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:3" ht="44" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>7</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>